<commit_message>
benchmark cigre residential/commercial/industrial added
</commit_message>
<xml_diff>
--- a/input_test/ele_profiles_commercial_cigre.xlsx
+++ b/input_test/ele_profiles_commercial_cigre.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24332"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\matti\OneDrive\Desktop\GIT\LoBi\input_dev\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pasqui\Desktop\GIT\LoBi\input_test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B927597-AC95-40C5-BCB8-665731F0ED23}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A5E3783-0683-40FB-908F-400ACE8E0BCB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17640" activeTab="11" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="1" sheetId="1" r:id="rId1"/>
@@ -138,7 +138,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normale" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -419,7 +419,7 @@
   <dimension ref="A1:I26"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="K18" sqref="K18"/>
+      <selection activeCell="J36" sqref="J36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -457,696 +457,696 @@
       <c r="A2" s="2">
         <v>0</v>
       </c>
-      <c r="B2" s="3">
-        <v>1</v>
-      </c>
-      <c r="C2" s="3">
-        <v>1</v>
-      </c>
-      <c r="D2" s="3">
-        <v>1</v>
-      </c>
-      <c r="E2" s="3">
-        <v>1</v>
-      </c>
-      <c r="F2" s="3">
-        <v>1</v>
-      </c>
-      <c r="G2" s="3">
-        <v>0.1</v>
-      </c>
-      <c r="H2" s="3">
-        <v>0.1</v>
-      </c>
-      <c r="I2" s="3">
-        <v>0.1</v>
+      <c r="B2">
+        <v>20.99</v>
+      </c>
+      <c r="C2">
+        <v>20.99</v>
+      </c>
+      <c r="D2">
+        <v>20.99</v>
+      </c>
+      <c r="E2">
+        <v>20.99</v>
+      </c>
+      <c r="F2">
+        <v>20.99</v>
+      </c>
+      <c r="G2">
+        <v>20.99</v>
+      </c>
+      <c r="H2">
+        <v>20.99</v>
+      </c>
+      <c r="I2">
+        <v>20.99</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>1</v>
       </c>
-      <c r="B3" s="3">
-        <v>1</v>
-      </c>
-      <c r="C3" s="3">
-        <v>1</v>
-      </c>
-      <c r="D3" s="3">
-        <v>1</v>
-      </c>
-      <c r="E3" s="3">
-        <v>1</v>
-      </c>
-      <c r="F3" s="3">
-        <v>1</v>
-      </c>
-      <c r="G3" s="3">
-        <v>0.1</v>
-      </c>
-      <c r="H3" s="3">
-        <v>0.1</v>
-      </c>
-      <c r="I3" s="3">
-        <v>0.1</v>
+      <c r="B3">
+        <v>20.25</v>
+      </c>
+      <c r="C3">
+        <v>20.25</v>
+      </c>
+      <c r="D3">
+        <v>20.25</v>
+      </c>
+      <c r="E3">
+        <v>20.25</v>
+      </c>
+      <c r="F3">
+        <v>20.25</v>
+      </c>
+      <c r="G3">
+        <v>20.25</v>
+      </c>
+      <c r="H3">
+        <v>20.25</v>
+      </c>
+      <c r="I3">
+        <v>20.25</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>2</v>
       </c>
-      <c r="B4" s="3">
-        <v>1</v>
-      </c>
-      <c r="C4" s="3">
-        <v>1</v>
-      </c>
-      <c r="D4" s="3">
-        <v>1</v>
-      </c>
-      <c r="E4" s="3">
-        <v>1</v>
-      </c>
-      <c r="F4" s="3">
-        <v>1</v>
-      </c>
-      <c r="G4" s="3">
-        <v>0.1</v>
-      </c>
-      <c r="H4" s="3">
-        <v>0.1</v>
-      </c>
-      <c r="I4" s="3">
-        <v>0.1</v>
+      <c r="B4">
+        <v>20.87</v>
+      </c>
+      <c r="C4">
+        <v>20.87</v>
+      </c>
+      <c r="D4">
+        <v>20.87</v>
+      </c>
+      <c r="E4">
+        <v>20.87</v>
+      </c>
+      <c r="F4">
+        <v>20.87</v>
+      </c>
+      <c r="G4">
+        <v>20.87</v>
+      </c>
+      <c r="H4">
+        <v>20.87</v>
+      </c>
+      <c r="I4">
+        <v>20.87</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>3</v>
       </c>
-      <c r="B5" s="3">
-        <v>1</v>
-      </c>
-      <c r="C5" s="3">
-        <v>1</v>
-      </c>
-      <c r="D5" s="3">
-        <v>1</v>
-      </c>
-      <c r="E5" s="3">
-        <v>1</v>
-      </c>
-      <c r="F5" s="3">
-        <v>1</v>
-      </c>
-      <c r="G5" s="3">
-        <v>0.1</v>
-      </c>
-      <c r="H5" s="3">
-        <v>0.1</v>
-      </c>
-      <c r="I5" s="3">
-        <v>0.1</v>
+      <c r="B5">
+        <v>21.74</v>
+      </c>
+      <c r="C5">
+        <v>21.74</v>
+      </c>
+      <c r="D5">
+        <v>21.74</v>
+      </c>
+      <c r="E5">
+        <v>21.74</v>
+      </c>
+      <c r="F5">
+        <v>21.74</v>
+      </c>
+      <c r="G5">
+        <v>21.74</v>
+      </c>
+      <c r="H5">
+        <v>21.74</v>
+      </c>
+      <c r="I5">
+        <v>21.74</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>4</v>
       </c>
-      <c r="B6" s="3">
-        <v>1</v>
-      </c>
-      <c r="C6" s="3">
-        <v>1</v>
-      </c>
-      <c r="D6" s="3">
-        <v>1</v>
-      </c>
-      <c r="E6" s="3">
-        <v>1</v>
-      </c>
-      <c r="F6" s="3">
-        <v>1</v>
-      </c>
-      <c r="G6" s="3">
-        <v>0.1</v>
-      </c>
-      <c r="H6" s="3">
-        <v>0.1</v>
-      </c>
-      <c r="I6" s="3">
-        <v>0.1</v>
+      <c r="B6">
+        <v>23.47</v>
+      </c>
+      <c r="C6">
+        <v>23.47</v>
+      </c>
+      <c r="D6">
+        <v>23.47</v>
+      </c>
+      <c r="E6">
+        <v>23.47</v>
+      </c>
+      <c r="F6">
+        <v>23.47</v>
+      </c>
+      <c r="G6">
+        <v>23.47</v>
+      </c>
+      <c r="H6">
+        <v>23.47</v>
+      </c>
+      <c r="I6">
+        <v>23.47</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>5</v>
       </c>
-      <c r="B7" s="3">
-        <v>1</v>
-      </c>
-      <c r="C7" s="3">
-        <v>1</v>
-      </c>
-      <c r="D7" s="3">
-        <v>1</v>
-      </c>
-      <c r="E7" s="3">
-        <v>1</v>
-      </c>
-      <c r="F7" s="3">
-        <v>1</v>
-      </c>
-      <c r="G7" s="3">
-        <v>0.1</v>
-      </c>
-      <c r="H7" s="3">
-        <v>0.1</v>
-      </c>
-      <c r="I7" s="3">
-        <v>0.1</v>
+      <c r="B7">
+        <v>25.46</v>
+      </c>
+      <c r="C7">
+        <v>25.46</v>
+      </c>
+      <c r="D7">
+        <v>25.46</v>
+      </c>
+      <c r="E7">
+        <v>25.46</v>
+      </c>
+      <c r="F7">
+        <v>25.46</v>
+      </c>
+      <c r="G7">
+        <v>25.46</v>
+      </c>
+      <c r="H7">
+        <v>25.46</v>
+      </c>
+      <c r="I7">
+        <v>25.46</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>6</v>
       </c>
-      <c r="B8" s="3">
-        <v>1</v>
-      </c>
-      <c r="C8" s="3">
-        <v>1</v>
-      </c>
-      <c r="D8" s="3">
-        <v>1</v>
-      </c>
-      <c r="E8" s="3">
-        <v>1</v>
-      </c>
-      <c r="F8" s="3">
-        <v>1</v>
-      </c>
-      <c r="G8" s="3">
-        <v>0.1</v>
-      </c>
-      <c r="H8" s="3">
-        <v>0.1</v>
-      </c>
-      <c r="I8" s="3">
-        <v>0.1</v>
+      <c r="B8">
+        <v>36.119999999999997</v>
+      </c>
+      <c r="C8">
+        <v>36.119999999999997</v>
+      </c>
+      <c r="D8">
+        <v>36.119999999999997</v>
+      </c>
+      <c r="E8">
+        <v>36.119999999999997</v>
+      </c>
+      <c r="F8">
+        <v>36.119999999999997</v>
+      </c>
+      <c r="G8">
+        <v>36.119999999999997</v>
+      </c>
+      <c r="H8">
+        <v>36.119999999999997</v>
+      </c>
+      <c r="I8">
+        <v>36.119999999999997</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <v>7</v>
       </c>
-      <c r="B9" s="3">
-        <v>1.2</v>
-      </c>
-      <c r="C9" s="3">
-        <v>1.2</v>
-      </c>
-      <c r="D9" s="3">
-        <v>1.2</v>
-      </c>
-      <c r="E9" s="3">
-        <v>1.2</v>
-      </c>
-      <c r="F9" s="3">
-        <v>1.2</v>
-      </c>
-      <c r="G9" s="3">
-        <v>0.1</v>
-      </c>
-      <c r="H9" s="3">
-        <v>0.1</v>
-      </c>
-      <c r="I9" s="3">
-        <v>0.1</v>
+      <c r="B9">
+        <v>49.27</v>
+      </c>
+      <c r="C9">
+        <v>49.27</v>
+      </c>
+      <c r="D9">
+        <v>49.27</v>
+      </c>
+      <c r="E9">
+        <v>49.27</v>
+      </c>
+      <c r="F9">
+        <v>49.27</v>
+      </c>
+      <c r="G9">
+        <v>49.27</v>
+      </c>
+      <c r="H9">
+        <v>49.27</v>
+      </c>
+      <c r="I9">
+        <v>49.27</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
         <v>8</v>
       </c>
-      <c r="B10" s="3">
-        <v>1.2</v>
-      </c>
-      <c r="C10" s="3">
-        <v>1.2</v>
-      </c>
-      <c r="D10" s="3">
-        <v>1.2</v>
-      </c>
-      <c r="E10" s="3">
-        <v>1.2</v>
-      </c>
-      <c r="F10" s="3">
-        <v>1.2</v>
-      </c>
-      <c r="G10" s="3">
-        <v>0.1</v>
-      </c>
-      <c r="H10" s="3">
-        <v>0.1</v>
-      </c>
-      <c r="I10" s="3">
-        <v>0.1</v>
+      <c r="B10">
+        <v>64.900000000000006</v>
+      </c>
+      <c r="C10">
+        <v>64.900000000000006</v>
+      </c>
+      <c r="D10">
+        <v>64.900000000000006</v>
+      </c>
+      <c r="E10">
+        <v>64.900000000000006</v>
+      </c>
+      <c r="F10">
+        <v>64.900000000000006</v>
+      </c>
+      <c r="G10">
+        <v>64.900000000000006</v>
+      </c>
+      <c r="H10">
+        <v>64.900000000000006</v>
+      </c>
+      <c r="I10">
+        <v>64.900000000000006</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
         <v>9</v>
       </c>
-      <c r="B11" s="3">
-        <v>1.2</v>
-      </c>
-      <c r="C11" s="3">
-        <v>1.2</v>
-      </c>
-      <c r="D11" s="3">
-        <v>1.2</v>
-      </c>
-      <c r="E11" s="3">
-        <v>1.2</v>
-      </c>
-      <c r="F11" s="3">
-        <v>1.2</v>
-      </c>
-      <c r="G11" s="3">
-        <v>0.1</v>
-      </c>
-      <c r="H11" s="3">
-        <v>0.1</v>
-      </c>
-      <c r="I11" s="3">
-        <v>0.1</v>
+      <c r="B11">
+        <v>79.41</v>
+      </c>
+      <c r="C11">
+        <v>79.41</v>
+      </c>
+      <c r="D11">
+        <v>79.41</v>
+      </c>
+      <c r="E11">
+        <v>79.41</v>
+      </c>
+      <c r="F11">
+        <v>79.41</v>
+      </c>
+      <c r="G11">
+        <v>79.41</v>
+      </c>
+      <c r="H11">
+        <v>79.41</v>
+      </c>
+      <c r="I11">
+        <v>79.41</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
         <v>10</v>
       </c>
-      <c r="B12" s="3">
-        <v>1.2</v>
-      </c>
-      <c r="C12" s="3">
-        <v>1.2</v>
-      </c>
-      <c r="D12" s="3">
-        <v>1.2</v>
-      </c>
-      <c r="E12" s="3">
-        <v>1.2</v>
-      </c>
-      <c r="F12" s="3">
-        <v>1.2</v>
-      </c>
-      <c r="G12" s="3">
-        <v>0.1</v>
-      </c>
-      <c r="H12" s="3">
-        <v>0.1</v>
-      </c>
-      <c r="I12" s="3">
-        <v>0.1</v>
+      <c r="B12">
+        <v>84.99</v>
+      </c>
+      <c r="C12">
+        <v>84.99</v>
+      </c>
+      <c r="D12">
+        <v>84.99</v>
+      </c>
+      <c r="E12">
+        <v>84.99</v>
+      </c>
+      <c r="F12">
+        <v>84.99</v>
+      </c>
+      <c r="G12">
+        <v>84.99</v>
+      </c>
+      <c r="H12">
+        <v>84.99</v>
+      </c>
+      <c r="I12">
+        <v>84.99</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
         <v>11</v>
       </c>
-      <c r="B13" s="3">
-        <v>1.2</v>
-      </c>
-      <c r="C13" s="3">
-        <v>1.2</v>
-      </c>
-      <c r="D13" s="3">
-        <v>1.2</v>
-      </c>
-      <c r="E13" s="3">
-        <v>1.2</v>
-      </c>
-      <c r="F13" s="3">
-        <v>1.2</v>
-      </c>
-      <c r="G13" s="3">
-        <v>0.1</v>
-      </c>
-      <c r="H13" s="3">
-        <v>0.1</v>
-      </c>
-      <c r="I13" s="3">
-        <v>0.1</v>
+      <c r="B13">
+        <v>89.83</v>
+      </c>
+      <c r="C13">
+        <v>89.83</v>
+      </c>
+      <c r="D13">
+        <v>89.83</v>
+      </c>
+      <c r="E13">
+        <v>89.83</v>
+      </c>
+      <c r="F13">
+        <v>89.83</v>
+      </c>
+      <c r="G13">
+        <v>89.83</v>
+      </c>
+      <c r="H13">
+        <v>89.83</v>
+      </c>
+      <c r="I13">
+        <v>89.83</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
         <v>12</v>
       </c>
-      <c r="B14" s="3">
-        <v>1.2</v>
-      </c>
-      <c r="C14" s="3">
-        <v>1.2</v>
-      </c>
-      <c r="D14" s="3">
-        <v>1.2</v>
-      </c>
-      <c r="E14" s="3">
-        <v>1.2</v>
-      </c>
-      <c r="F14" s="3">
-        <v>1.2</v>
-      </c>
-      <c r="G14" s="3">
-        <v>0.1</v>
-      </c>
-      <c r="H14" s="3">
-        <v>0.1</v>
-      </c>
-      <c r="I14" s="3">
-        <v>0.1</v>
+      <c r="B14">
+        <v>92.31</v>
+      </c>
+      <c r="C14">
+        <v>92.31</v>
+      </c>
+      <c r="D14">
+        <v>92.31</v>
+      </c>
+      <c r="E14">
+        <v>92.31</v>
+      </c>
+      <c r="F14">
+        <v>92.31</v>
+      </c>
+      <c r="G14">
+        <v>92.31</v>
+      </c>
+      <c r="H14">
+        <v>92.31</v>
+      </c>
+      <c r="I14">
+        <v>92.31</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
         <v>13</v>
       </c>
-      <c r="B15" s="3">
-        <v>1.2</v>
-      </c>
-      <c r="C15" s="3">
-        <v>1.2</v>
-      </c>
-      <c r="D15" s="3">
-        <v>1.2</v>
-      </c>
-      <c r="E15" s="3">
-        <v>1.2</v>
-      </c>
-      <c r="F15" s="3">
-        <v>1.2</v>
-      </c>
-      <c r="G15" s="3">
-        <v>0.1</v>
-      </c>
-      <c r="H15" s="3">
-        <v>0.1</v>
-      </c>
-      <c r="I15" s="3">
-        <v>0.1</v>
+      <c r="B15">
+        <v>91.94</v>
+      </c>
+      <c r="C15">
+        <v>91.94</v>
+      </c>
+      <c r="D15">
+        <v>91.94</v>
+      </c>
+      <c r="E15">
+        <v>91.94</v>
+      </c>
+      <c r="F15">
+        <v>91.94</v>
+      </c>
+      <c r="G15">
+        <v>91.94</v>
+      </c>
+      <c r="H15">
+        <v>91.94</v>
+      </c>
+      <c r="I15">
+        <v>91.94</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="2">
         <v>14</v>
       </c>
-      <c r="B16" s="3">
-        <v>1.2</v>
-      </c>
-      <c r="C16" s="3">
-        <v>1.2</v>
-      </c>
-      <c r="D16" s="3">
-        <v>1.2</v>
-      </c>
-      <c r="E16" s="3">
-        <v>1.2</v>
-      </c>
-      <c r="F16" s="3">
-        <v>1.2</v>
-      </c>
-      <c r="G16" s="3">
-        <v>0.1</v>
-      </c>
-      <c r="H16" s="3">
-        <v>0.1</v>
-      </c>
-      <c r="I16" s="3">
-        <v>0.1</v>
+      <c r="B16">
+        <v>87.6</v>
+      </c>
+      <c r="C16">
+        <v>87.6</v>
+      </c>
+      <c r="D16">
+        <v>87.6</v>
+      </c>
+      <c r="E16">
+        <v>87.6</v>
+      </c>
+      <c r="F16">
+        <v>87.6</v>
+      </c>
+      <c r="G16">
+        <v>87.6</v>
+      </c>
+      <c r="H16">
+        <v>87.6</v>
+      </c>
+      <c r="I16">
+        <v>87.6</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="2">
         <v>15</v>
       </c>
-      <c r="B17" s="3">
-        <v>1.2</v>
-      </c>
-      <c r="C17" s="3">
-        <v>1.2</v>
-      </c>
-      <c r="D17" s="3">
-        <v>1.2</v>
-      </c>
-      <c r="E17" s="3">
-        <v>1.2</v>
-      </c>
-      <c r="F17" s="3">
-        <v>1.2</v>
-      </c>
-      <c r="G17" s="3">
-        <v>0.1</v>
-      </c>
-      <c r="H17" s="3">
-        <v>0.1</v>
-      </c>
-      <c r="I17" s="3">
-        <v>0.1</v>
+      <c r="B17">
+        <v>85.61</v>
+      </c>
+      <c r="C17">
+        <v>85.61</v>
+      </c>
+      <c r="D17">
+        <v>85.61</v>
+      </c>
+      <c r="E17">
+        <v>85.61</v>
+      </c>
+      <c r="F17">
+        <v>85.61</v>
+      </c>
+      <c r="G17">
+        <v>85.61</v>
+      </c>
+      <c r="H17">
+        <v>85.61</v>
+      </c>
+      <c r="I17">
+        <v>85.61</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="2">
         <v>16</v>
       </c>
-      <c r="B18" s="3">
-        <v>1.2</v>
-      </c>
-      <c r="C18" s="3">
-        <v>1.2</v>
-      </c>
-      <c r="D18" s="3">
-        <v>1.2</v>
-      </c>
-      <c r="E18" s="3">
-        <v>1.2</v>
-      </c>
-      <c r="F18" s="3">
-        <v>1.2</v>
-      </c>
-      <c r="G18" s="3">
-        <v>0.1</v>
-      </c>
-      <c r="H18" s="3">
-        <v>0.1</v>
-      </c>
-      <c r="I18" s="3">
-        <v>0.1</v>
+      <c r="B18">
+        <v>89.83</v>
+      </c>
+      <c r="C18">
+        <v>89.83</v>
+      </c>
+      <c r="D18">
+        <v>89.83</v>
+      </c>
+      <c r="E18">
+        <v>89.83</v>
+      </c>
+      <c r="F18">
+        <v>89.83</v>
+      </c>
+      <c r="G18">
+        <v>89.83</v>
+      </c>
+      <c r="H18">
+        <v>89.83</v>
+      </c>
+      <c r="I18">
+        <v>89.83</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" s="2">
         <v>17</v>
       </c>
-      <c r="B19" s="3">
-        <v>1.2</v>
-      </c>
-      <c r="C19" s="3">
-        <v>1.2</v>
-      </c>
-      <c r="D19" s="3">
-        <v>1.2</v>
-      </c>
-      <c r="E19" s="3">
-        <v>1.2</v>
-      </c>
-      <c r="F19" s="3">
-        <v>1.2</v>
-      </c>
-      <c r="G19" s="3">
-        <v>0.1</v>
-      </c>
-      <c r="H19" s="3">
-        <v>0.1</v>
-      </c>
-      <c r="I19" s="3">
-        <v>0.1</v>
+      <c r="B19">
+        <v>99.75</v>
+      </c>
+      <c r="C19">
+        <v>99.75</v>
+      </c>
+      <c r="D19">
+        <v>99.75</v>
+      </c>
+      <c r="E19">
+        <v>99.75</v>
+      </c>
+      <c r="F19">
+        <v>99.75</v>
+      </c>
+      <c r="G19">
+        <v>99.75</v>
+      </c>
+      <c r="H19">
+        <v>99.75</v>
+      </c>
+      <c r="I19">
+        <v>99.75</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" s="2">
         <v>18</v>
       </c>
-      <c r="B20" s="3">
-        <v>1.2</v>
-      </c>
-      <c r="C20" s="3">
-        <v>1.2</v>
-      </c>
-      <c r="D20" s="3">
-        <v>1.2</v>
-      </c>
-      <c r="E20" s="3">
-        <v>1.2</v>
-      </c>
-      <c r="F20" s="3">
-        <v>1.2</v>
-      </c>
-      <c r="G20" s="3">
-        <v>0.1</v>
-      </c>
-      <c r="H20" s="3">
-        <v>0.1</v>
-      </c>
-      <c r="I20" s="3">
-        <v>0.1</v>
+      <c r="B20">
+        <v>79.66</v>
+      </c>
+      <c r="C20">
+        <v>79.66</v>
+      </c>
+      <c r="D20">
+        <v>79.66</v>
+      </c>
+      <c r="E20">
+        <v>79.66</v>
+      </c>
+      <c r="F20">
+        <v>79.66</v>
+      </c>
+      <c r="G20">
+        <v>79.66</v>
+      </c>
+      <c r="H20">
+        <v>79.66</v>
+      </c>
+      <c r="I20">
+        <v>79.66</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" s="2">
         <v>19</v>
       </c>
-      <c r="B21" s="3">
-        <v>1</v>
-      </c>
-      <c r="C21" s="3">
-        <v>1</v>
-      </c>
-      <c r="D21" s="3">
-        <v>1</v>
-      </c>
-      <c r="E21" s="3">
-        <v>1</v>
-      </c>
-      <c r="F21" s="3">
-        <v>1</v>
-      </c>
-      <c r="G21" s="3">
-        <v>0.1</v>
-      </c>
-      <c r="H21" s="3">
-        <v>0.1</v>
-      </c>
-      <c r="I21" s="3">
-        <v>0.1</v>
+      <c r="B21">
+        <v>69.98</v>
+      </c>
+      <c r="C21">
+        <v>69.98</v>
+      </c>
+      <c r="D21">
+        <v>69.98</v>
+      </c>
+      <c r="E21">
+        <v>69.98</v>
+      </c>
+      <c r="F21">
+        <v>69.98</v>
+      </c>
+      <c r="G21">
+        <v>69.98</v>
+      </c>
+      <c r="H21">
+        <v>69.98</v>
+      </c>
+      <c r="I21">
+        <v>69.98</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" s="2">
         <v>20</v>
       </c>
-      <c r="B22" s="3">
-        <v>1</v>
-      </c>
-      <c r="C22" s="3">
-        <v>1</v>
-      </c>
-      <c r="D22" s="3">
-        <v>1</v>
-      </c>
-      <c r="E22" s="3">
-        <v>1</v>
-      </c>
-      <c r="F22" s="3">
-        <v>1</v>
-      </c>
-      <c r="G22" s="3">
-        <v>0.1</v>
-      </c>
-      <c r="H22" s="3">
-        <v>0.1</v>
-      </c>
-      <c r="I22" s="3">
-        <v>0.1</v>
+      <c r="B22">
+        <v>59.19</v>
+      </c>
+      <c r="C22">
+        <v>59.19</v>
+      </c>
+      <c r="D22">
+        <v>59.19</v>
+      </c>
+      <c r="E22">
+        <v>59.19</v>
+      </c>
+      <c r="F22">
+        <v>59.19</v>
+      </c>
+      <c r="G22">
+        <v>59.19</v>
+      </c>
+      <c r="H22">
+        <v>59.19</v>
+      </c>
+      <c r="I22">
+        <v>59.19</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" s="2">
         <v>21</v>
       </c>
-      <c r="B23" s="3">
-        <v>1</v>
-      </c>
-      <c r="C23" s="3">
-        <v>1</v>
-      </c>
-      <c r="D23" s="3">
-        <v>1</v>
-      </c>
-      <c r="E23" s="3">
-        <v>1</v>
-      </c>
-      <c r="F23" s="3">
-        <v>1</v>
-      </c>
-      <c r="G23" s="3">
-        <v>0.1</v>
-      </c>
-      <c r="H23" s="3">
-        <v>0.1</v>
-      </c>
-      <c r="I23" s="3">
-        <v>0.1</v>
+      <c r="B23">
+        <v>48.9</v>
+      </c>
+      <c r="C23">
+        <v>48.9</v>
+      </c>
+      <c r="D23">
+        <v>48.9</v>
+      </c>
+      <c r="E23">
+        <v>48.9</v>
+      </c>
+      <c r="F23">
+        <v>48.9</v>
+      </c>
+      <c r="G23">
+        <v>48.9</v>
+      </c>
+      <c r="H23">
+        <v>48.9</v>
+      </c>
+      <c r="I23">
+        <v>48.9</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" s="2">
         <v>22</v>
       </c>
-      <c r="B24" s="3">
-        <v>1</v>
-      </c>
-      <c r="C24" s="3">
-        <v>1</v>
-      </c>
-      <c r="D24" s="3">
-        <v>1</v>
-      </c>
-      <c r="E24" s="3">
-        <v>1</v>
-      </c>
-      <c r="F24" s="3">
-        <v>1</v>
-      </c>
-      <c r="G24" s="3">
-        <v>0.1</v>
-      </c>
-      <c r="H24" s="3">
-        <v>0.1</v>
-      </c>
-      <c r="I24" s="3">
-        <v>0.1</v>
+      <c r="B24">
+        <v>29.92</v>
+      </c>
+      <c r="C24">
+        <v>29.92</v>
+      </c>
+      <c r="D24">
+        <v>29.92</v>
+      </c>
+      <c r="E24">
+        <v>29.92</v>
+      </c>
+      <c r="F24">
+        <v>29.92</v>
+      </c>
+      <c r="G24">
+        <v>29.92</v>
+      </c>
+      <c r="H24">
+        <v>29.92</v>
+      </c>
+      <c r="I24">
+        <v>29.92</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" s="2">
         <v>23</v>
       </c>
-      <c r="B25" s="3">
-        <v>1</v>
-      </c>
-      <c r="C25" s="3">
-        <v>1</v>
-      </c>
-      <c r="D25" s="3">
-        <v>1</v>
-      </c>
-      <c r="E25" s="3">
-        <v>1</v>
-      </c>
-      <c r="F25" s="3">
-        <v>1</v>
-      </c>
-      <c r="G25" s="3">
-        <v>0.1</v>
-      </c>
-      <c r="H25" s="3">
-        <v>0.1</v>
-      </c>
-      <c r="I25" s="3">
-        <v>0.1</v>
+      <c r="B25">
+        <v>19.75</v>
+      </c>
+      <c r="C25">
+        <v>19.75</v>
+      </c>
+      <c r="D25">
+        <v>19.75</v>
+      </c>
+      <c r="E25">
+        <v>19.75</v>
+      </c>
+      <c r="F25">
+        <v>19.75</v>
+      </c>
+      <c r="G25">
+        <v>19.75</v>
+      </c>
+      <c r="H25">
+        <v>19.75</v>
+      </c>
+      <c r="I25">
+        <v>19.75</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
@@ -2641,7 +2641,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{93B4A697-4844-4049-82F3-64202AF8B0B4}">
   <dimension ref="A1:I25"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="K18" sqref="K18"/>
     </sheetView>
   </sheetViews>
@@ -3382,7 +3382,7 @@
   <dimension ref="A1:I25"/>
   <sheetViews>
     <sheetView zoomScale="74" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:I25"/>
+      <selection activeCell="I25" sqref="B2:I25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6341,8 +6341,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8A834683-A25B-40D6-9D5E-CCDEA83103D1}">
   <dimension ref="A1:I25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:I25"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F35" sqref="F35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>